<commit_message>
lc desktop accg1000 & comp2250 assignments
</commit_message>
<xml_diff>
--- a/2021/S3/COMP2250/Assignment 1/Assignment 1, Task B.xlsx
+++ b/2021/S3/COMP2250/Assignment 1/Assignment 1, Task B.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAI_CAREY\Desktop\Uni\COMP2250\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAI_CAREY\Desktop\Uni\2021\S3\COMP2250\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC1DEE0-CBA7-45F2-97DD-53C7E454FEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9C2D19-5635-4802-AAFC-EAECF0B4873D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{88C157EC-67CF-41F6-A806-D45A0CEF2632}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88C157EC-67CF-41F6-A806-D45A0CEF2632}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
   <si>
     <t>Subnet Number</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>175.21.255.255</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Usable</t>
   </si>
 </sst>
 </file>
@@ -335,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -343,23 +352,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -678,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D9CB3C-5C05-42DD-9A4F-ED8856285B3E}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,60 +746,64 @@
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -758,16 +818,18 @@
       <c r="E3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -782,16 +844,18 @@
       <c r="E4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -806,16 +870,18 @@
       <c r="E5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -830,16 +896,18 @@
       <c r="E6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -854,16 +922,18 @@
       <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -878,16 +948,18 @@
       <c r="E8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -902,16 +974,18 @@
       <c r="E9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -926,15 +1000,18 @@
       <c r="E10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="H10" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -949,15 +1026,18 @@
       <c r="E11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="H11" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -972,15 +1052,18 @@
       <c r="E12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -995,15 +1078,18 @@
       <c r="E13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="H13" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1018,15 +1104,18 @@
       <c r="E14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="3" t="s">
         <v>81</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1041,15 +1130,18 @@
       <c r="E15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="H15" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1064,15 +1156,18 @@
       <c r="E16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="H16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1087,11 +1182,14 @@
       <c r="E17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>87</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>